<commit_message>
added fine time resolution of observations to xlsx file and script
</commit_message>
<xml_diff>
--- a/DATA/Pulsars_fluxes.xlsx
+++ b/DATA/Pulsars_fluxes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>2019.11.03</t>
+  </si>
+  <si>
+    <t>temp resolution GURT</t>
+  </si>
+  <si>
+    <t>temp resolution UTR2</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +229,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -236,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -257,6 +269,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,622 +550,706 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O12" sqref="O12"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="3" customWidth="1"/>
+    <col min="1" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="9" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" style="7" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="9" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" style="7" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="7" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="5" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" style="3" customWidth="1"/>
     <col min="18" max="18" width="12.7109375" style="5" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" style="9" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" style="7" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="5" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" style="3" customWidth="1"/>
     <col min="22" max="22" width="12.7109375" style="9" customWidth="1"/>
     <col min="23" max="23" width="12.7109375" style="7" customWidth="1"/>
     <col min="24" max="24" width="12.7109375" style="9" customWidth="1"/>
     <col min="25" max="25" width="12.7109375" style="7" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" style="9" customWidth="1"/>
+    <col min="27" max="27" width="12.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="9">
+      <c r="B2">
+        <v>9.83</v>
+      </c>
+      <c r="C2">
+        <v>7.94</v>
+      </c>
+      <c r="J2" s="9">
         <v>11.9</v>
       </c>
-      <c r="I2" s="7">
+      <c r="K2" s="7">
         <v>114.5</v>
       </c>
-      <c r="M2" s="7">
+      <c r="O2" s="7">
         <v>4.8491</v>
       </c>
-      <c r="N2" s="5">
+      <c r="P2" s="5">
         <v>17.2</v>
       </c>
-      <c r="O2" s="3">
+      <c r="Q2" s="3">
         <v>13.3</v>
       </c>
-      <c r="S2" s="3">
+      <c r="U2" s="3">
         <v>19.631</v>
       </c>
-      <c r="T2" s="9">
+      <c r="V2" s="9">
         <v>34</v>
       </c>
-      <c r="U2" s="7">
+      <c r="W2" s="7">
         <v>196.1</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="AA2" s="7">
         <v>12.4429</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="9">
+      <c r="B3">
+        <v>9.83</v>
+      </c>
+      <c r="C3">
+        <v>7.94</v>
+      </c>
+      <c r="J3" s="9">
         <v>12.6</v>
       </c>
-      <c r="I3" s="7">
+      <c r="K3" s="7">
         <v>94.6</v>
       </c>
-      <c r="M3" s="7">
+      <c r="O3" s="7">
         <v>4.8491</v>
       </c>
-      <c r="N3" s="5">
+      <c r="P3" s="5">
         <v>16.100000000000001</v>
       </c>
-      <c r="O3" s="3">
+      <c r="Q3" s="3">
         <v>14.6</v>
       </c>
-      <c r="S3" s="3">
+      <c r="U3" s="3">
         <v>19.625</v>
       </c>
-      <c r="T3" s="9">
+      <c r="V3" s="9">
         <v>-1</v>
       </c>
-      <c r="U3" s="7">
+      <c r="W3" s="7">
         <v>202.4</v>
       </c>
-      <c r="Y3" s="7">
+      <c r="AA3" s="7">
         <v>12.444900000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="9">
+      <c r="B4">
+        <v>9.83</v>
+      </c>
+      <c r="C4">
+        <v>7.94</v>
+      </c>
+      <c r="J4" s="9">
         <v>12.4</v>
       </c>
-      <c r="I4" s="7">
+      <c r="K4" s="7">
         <v>178.1</v>
       </c>
-      <c r="M4" s="7">
+      <c r="O4" s="7">
         <v>4.8491</v>
       </c>
-      <c r="N4" s="5">
+      <c r="P4" s="5">
         <v>20.100000000000001</v>
       </c>
-      <c r="O4" s="3">
+      <c r="Q4" s="3">
         <v>13.5</v>
       </c>
-      <c r="S4" s="3">
+      <c r="U4" s="3">
         <v>19.626999999999999</v>
       </c>
-      <c r="T4" s="9">
+      <c r="V4" s="9">
         <v>42</v>
       </c>
-      <c r="U4" s="7">
+      <c r="W4" s="7">
         <v>235.5</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="AA4" s="7">
         <v>12.444900000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="9">
+      <c r="B5">
+        <v>9.83</v>
+      </c>
+      <c r="C5">
+        <v>7.94</v>
+      </c>
+      <c r="J5" s="9">
         <v>12.2</v>
       </c>
-      <c r="I5" s="7">
+      <c r="K5" s="7">
         <v>217.6</v>
       </c>
-      <c r="M5" s="7">
+      <c r="O5" s="7">
         <v>4.8491</v>
       </c>
-      <c r="N5" s="5">
+      <c r="P5" s="5">
         <v>18.7</v>
       </c>
-      <c r="O5" s="3">
+      <c r="Q5" s="3">
         <v>12.3</v>
       </c>
-      <c r="S5" s="3">
+      <c r="U5" s="3">
         <v>19.625</v>
       </c>
-      <c r="T5" s="9">
+      <c r="V5" s="9">
         <v>40.799999999999997</v>
       </c>
-      <c r="U5" s="7">
+      <c r="W5" s="7">
         <v>231.5</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="AA5" s="7">
         <v>12.444900000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="9">
+      <c r="B6">
+        <v>9.83</v>
+      </c>
+      <c r="C6">
+        <v>7.94</v>
+      </c>
+      <c r="J6" s="9">
         <v>13.7</v>
       </c>
-      <c r="I6" s="7">
+      <c r="K6" s="7">
         <v>62.8</v>
       </c>
-      <c r="M6" s="7">
+      <c r="O6" s="7">
         <v>4.8471000000000002</v>
       </c>
-      <c r="N6" s="5">
+      <c r="P6" s="5">
         <v>14.2</v>
       </c>
-      <c r="O6" s="3">
+      <c r="Q6" s="3">
         <v>9.8000000000000007</v>
       </c>
-      <c r="S6" s="3">
+      <c r="U6" s="3">
         <v>19.617000000000001</v>
       </c>
-      <c r="T6" s="9">
+      <c r="V6" s="9">
         <v>46.5</v>
       </c>
-      <c r="U6" s="7">
+      <c r="W6" s="7">
         <v>215.1</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="AA6" s="7">
         <v>12.444900000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="9">
+      <c r="B7">
+        <v>9.83</v>
+      </c>
+      <c r="C7">
+        <v>7.94</v>
+      </c>
+      <c r="J7" s="9">
         <v>12.9</v>
       </c>
-      <c r="I7" s="7">
+      <c r="K7" s="7">
         <v>188.5</v>
       </c>
-      <c r="M7" s="7">
+      <c r="O7" s="7">
         <v>-1</v>
       </c>
-      <c r="O7" s="3">
+      <c r="Q7" s="3">
         <v>15.3</v>
       </c>
-      <c r="S7" s="3">
+      <c r="U7" s="3">
         <v>-1</v>
       </c>
-      <c r="T7" s="9">
+      <c r="V7" s="9">
         <v>42</v>
       </c>
-      <c r="U7" s="7">
+      <c r="W7" s="7">
         <v>209.3</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="AA7" s="7">
         <v>12.444900000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="9">
+      <c r="B8">
+        <v>9.83</v>
+      </c>
+      <c r="C8">
+        <v>7.94</v>
+      </c>
+      <c r="J8" s="9">
         <v>11.9</v>
       </c>
-      <c r="I8" s="7">
+      <c r="K8" s="7">
         <v>129.6</v>
       </c>
-      <c r="M8" s="7">
+      <c r="O8" s="7">
         <v>4.8471000000000002</v>
       </c>
-      <c r="N8" s="5">
+      <c r="P8" s="5">
         <v>19.5</v>
       </c>
-      <c r="O8" s="3">
+      <c r="Q8" s="3">
         <v>12.9</v>
       </c>
-      <c r="S8" s="3">
+      <c r="U8" s="3">
         <v>19.623000000000001</v>
       </c>
-      <c r="T8" s="9">
+      <c r="V8" s="9">
         <v>42.1</v>
       </c>
-      <c r="U8" s="7">
+      <c r="W8" s="7">
         <v>238.1</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="AA8" s="7">
         <v>12.444900000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="9">
+      <c r="B9">
+        <v>9.83</v>
+      </c>
+      <c r="C9">
+        <v>7.94</v>
+      </c>
+      <c r="J9" s="9">
         <v>15.6</v>
       </c>
-      <c r="I9" s="7">
+      <c r="K9" s="7">
         <v>182.8</v>
       </c>
-      <c r="M9" s="7">
+      <c r="O9" s="7">
         <v>4.8471000000000002</v>
       </c>
-      <c r="N9" s="5">
+      <c r="P9" s="5">
         <v>23</v>
       </c>
-      <c r="O9" s="3">
+      <c r="Q9" s="3">
         <v>15.7</v>
       </c>
-      <c r="S9" s="3">
+      <c r="U9" s="3">
         <v>19.626999999999999</v>
       </c>
-      <c r="T9" s="9">
+      <c r="V9" s="9">
         <v>36</v>
       </c>
-      <c r="U9" s="7">
+      <c r="W9" s="7">
         <v>164.2</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="AA9" s="7">
         <v>12.4429</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="9">
+      <c r="B10">
+        <v>9.83</v>
+      </c>
+      <c r="C10">
+        <v>7.94</v>
+      </c>
+      <c r="J10" s="9">
         <v>18.600000000000001</v>
       </c>
-      <c r="I10" s="7">
+      <c r="K10" s="7">
         <v>159.19999999999999</v>
       </c>
-      <c r="J10" s="9">
+      <c r="L10" s="9">
         <v>24.5</v>
       </c>
-      <c r="K10" s="7">
+      <c r="M10" s="7">
         <v>22.9</v>
       </c>
-      <c r="M10" s="7">
+      <c r="O10" s="7">
         <v>4.8471000000000002</v>
       </c>
-      <c r="N10" s="5">
+      <c r="P10" s="5">
         <v>16.8</v>
-      </c>
-      <c r="O10" s="3">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
-        <v>0</v>
       </c>
       <c r="Q10" s="3">
         <v>0</v>
       </c>
+      <c r="R10" s="5">
+        <v>0</v>
+      </c>
       <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="U10" s="3">
         <v>-1</v>
       </c>
-      <c r="T10" s="9">
+      <c r="V10" s="9">
         <v>46.9</v>
       </c>
-      <c r="U10" s="7">
+      <c r="W10" s="7">
         <v>7.4</v>
       </c>
-      <c r="V10" s="9">
+      <c r="X10" s="9">
         <v>0</v>
       </c>
-      <c r="W10" s="7">
+      <c r="Y10" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="AA10" s="7">
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="9">
+      <c r="B11">
+        <v>9.83</v>
+      </c>
+      <c r="C11">
+        <v>7.94</v>
+      </c>
+      <c r="J11" s="9">
         <v>21</v>
       </c>
-      <c r="I11" s="7">
+      <c r="K11" s="7">
         <v>137.9</v>
       </c>
-      <c r="J11" s="9">
+      <c r="L11" s="9">
         <v>24.8</v>
       </c>
-      <c r="K11" s="7">
+      <c r="M11" s="7">
         <v>13.7</v>
       </c>
-      <c r="M11" s="7">
+      <c r="O11" s="7">
         <v>4.8491</v>
       </c>
-      <c r="N11" s="5">
+      <c r="P11" s="5">
         <v>11.2</v>
       </c>
-      <c r="O11" s="3">
+      <c r="Q11" s="3">
         <v>24.5</v>
       </c>
-      <c r="P11" s="5">
+      <c r="R11" s="5">
         <v>2.8</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="S11" s="3">
         <v>4.5</v>
       </c>
-      <c r="S11" s="3">
+      <c r="U11" s="3">
         <v>19.631</v>
       </c>
-      <c r="T11" s="9">
+      <c r="V11" s="9">
         <v>49</v>
       </c>
-      <c r="U11" s="7">
+      <c r="W11" s="7">
         <v>10.1</v>
       </c>
-      <c r="V11" s="9">
+      <c r="X11" s="9">
         <v>0</v>
       </c>
-      <c r="W11" s="7">
+      <c r="Y11" s="7">
         <v>8.6</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="AA11" s="7">
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="9">
+      <c r="B12">
+        <v>9.83</v>
+      </c>
+      <c r="C12">
+        <v>7.94</v>
+      </c>
+      <c r="J12" s="9">
         <v>16.5</v>
       </c>
-      <c r="I12" s="7">
+      <c r="K12" s="7">
         <v>143.4</v>
       </c>
-      <c r="J12" s="9">
+      <c r="L12" s="9">
         <v>25.3</v>
       </c>
-      <c r="K12" s="7">
+      <c r="M12" s="7">
         <v>17</v>
       </c>
-      <c r="M12" s="7">
+      <c r="O12" s="7">
         <v>4.8491</v>
       </c>
-      <c r="N12" s="5">
+      <c r="P12" s="5">
         <v>9.4</v>
       </c>
-      <c r="O12" s="3">
+      <c r="Q12" s="3">
         <v>24</v>
       </c>
-      <c r="P12" s="5">
+      <c r="R12" s="5">
         <v>3.3</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="S12" s="3">
         <v>4.3</v>
       </c>
-      <c r="S12" s="3">
+      <c r="U12" s="3">
         <v>19.623000000000001</v>
       </c>
-      <c r="T12" s="9">
+      <c r="V12" s="9">
         <v>44.8</v>
       </c>
-      <c r="U12" s="7">
+      <c r="W12" s="7">
         <v>225.8</v>
       </c>
-      <c r="V12" s="9">
+      <c r="X12" s="9">
         <v>29.6</v>
       </c>
-      <c r="W12" s="7">
+      <c r="Y12" s="7">
         <v>21.7</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="AA12" s="7">
         <v>12.4429</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="9">
+      <c r="B13">
+        <v>9.83</v>
+      </c>
+      <c r="C13">
+        <v>7.94</v>
+      </c>
+      <c r="J13" s="9">
         <v>10.5</v>
       </c>
-      <c r="I13" s="7">
+      <c r="K13" s="7">
         <v>158.80000000000001</v>
       </c>
-      <c r="J13" s="9">
+      <c r="L13" s="9">
         <v>28.6</v>
       </c>
-      <c r="K13" s="7">
+      <c r="M13" s="7">
         <v>15.8</v>
       </c>
-      <c r="M13" s="7">
+      <c r="O13" s="7">
         <v>4.8471000000000002</v>
       </c>
-      <c r="O13" s="3">
+      <c r="Q13" s="3">
         <v>26.7</v>
       </c>
-      <c r="P13" s="5">
+      <c r="R13" s="5">
         <v>5.2</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="S13" s="3">
         <v>0</v>
       </c>
-      <c r="S13" s="3">
+      <c r="U13" s="3">
         <v>-1</v>
       </c>
-      <c r="T13" s="9">
+      <c r="V13" s="9">
         <v>-1</v>
       </c>
-      <c r="U13" s="7">
+      <c r="W13" s="7">
         <v>236.9</v>
       </c>
-      <c r="V13" s="9">
+      <c r="X13" s="9">
         <v>23.4</v>
       </c>
-      <c r="W13" s="7">
+      <c r="Y13" s="7">
         <v>21.1</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="AA13" s="7">
         <v>12.444900000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="9">
+      <c r="B14">
+        <v>9.83</v>
+      </c>
+      <c r="C14">
+        <v>7.94</v>
+      </c>
+      <c r="J14" s="9">
         <v>13</v>
       </c>
-      <c r="I14" s="7">
+      <c r="K14" s="7">
         <v>147.19999999999999</v>
       </c>
-      <c r="J14" s="9">
+      <c r="L14" s="9">
         <v>26.3</v>
       </c>
-      <c r="K14" s="7">
+      <c r="M14" s="7">
         <v>16.8</v>
       </c>
-      <c r="M14" s="7">
+      <c r="O14" s="7">
         <v>-1</v>
       </c>
-      <c r="O14" s="3">
+      <c r="Q14" s="3">
         <v>25.4</v>
       </c>
-      <c r="P14" s="5">
+      <c r="R14" s="5">
         <v>5.2</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="S14" s="3">
         <v>0</v>
       </c>
-      <c r="S14" s="3">
+      <c r="U14" s="3">
         <v>-1</v>
       </c>
-      <c r="T14" s="9">
+      <c r="V14" s="9">
         <v>-1</v>
       </c>
-      <c r="U14" s="7">
+      <c r="W14" s="7">
         <v>6.9</v>
       </c>
-      <c r="V14" s="9">
+      <c r="X14" s="9">
         <v>0</v>
       </c>
-      <c r="W14" s="7">
+      <c r="Y14" s="7">
         <v>7.2</v>
       </c>
-      <c r="Y14" s="7">
+      <c r="AA14" s="7">
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added first batch of new data
</commit_message>
<xml_diff>
--- a/DATA/Pulsars_fluxes.xlsx
+++ b/DATA/Pulsars_fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\python\jupyter-radio-astronomy\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PYTHON\jupyter-radio-astronomy\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -574,7 +574,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E7" sqref="E7"/>
+      <selection pane="topRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,65 +1270,212 @@
       <c r="A15" t="s">
         <v>38</v>
       </c>
+      <c r="C15" s="14">
+        <v>7.94</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" s="14">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" s="14">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" s="14">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" s="14">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C20" s="14">
+        <v>7.94</v>
+      </c>
+      <c r="E20" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="F20" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="H20" s="5">
+        <v>10.894</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" s="14">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22" s="14">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C23" s="14">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C24" s="14">
+        <v>7.94</v>
+      </c>
+      <c r="K24" s="7">
+        <v>94.6</v>
+      </c>
+      <c r="N24" s="9">
+        <v>4.8471000000000002</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>11.5</v>
+      </c>
+      <c r="T24" s="5">
+        <v>19.623000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C25" s="14">
+        <v>7.94</v>
+      </c>
+      <c r="E25" s="3">
+        <v>13.6</v>
+      </c>
+      <c r="F25" s="5">
+        <v>10.8</v>
+      </c>
+      <c r="H25" s="5">
+        <v>10.896000000000001</v>
+      </c>
+      <c r="K25" s="7">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="L25" s="9">
+        <v>18.2</v>
+      </c>
+      <c r="N25" s="9">
+        <v>4.8471000000000002</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>55.2</v>
+      </c>
+      <c r="R25" s="5">
+        <v>10.4</v>
+      </c>
+      <c r="T25" s="5">
+        <v>19.623000000000001</v>
+      </c>
+      <c r="W25" s="7">
+        <v>253.9</v>
+      </c>
+      <c r="X25" s="9">
+        <v>51</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>12.440899999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C26" s="14">
+        <v>7.94</v>
+      </c>
+      <c r="E26" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="H26" s="5">
+        <v>10.896000000000001</v>
+      </c>
+      <c r="K26" s="7">
+        <v>90.8</v>
+      </c>
+      <c r="L26" s="9">
+        <v>19.8</v>
+      </c>
+      <c r="N26" s="9">
+        <v>4.8471000000000002</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>43.5</v>
+      </c>
+      <c r="R26" s="5">
+        <v>10.6</v>
+      </c>
+      <c r="T26" s="5">
+        <v>19.619</v>
+      </c>
+      <c r="W26" s="7">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="X26" s="9">
+        <v>48</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>12.4429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
+      </c>
+      <c r="C27" s="14">
+        <v>7.94</v>
+      </c>
+      <c r="E27" s="3">
+        <v>12.6</v>
+      </c>
+      <c r="F27" s="5">
+        <v>6.9</v>
+      </c>
+      <c r="H27" s="5">
+        <v>10.894</v>
+      </c>
+      <c r="K27" s="7">
+        <v>88.5</v>
+      </c>
+      <c r="L27" s="9">
+        <v>19.3</v>
+      </c>
+      <c r="N27" s="9">
+        <v>4.8471000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added plots for DM and specral index
</commit_message>
<xml_diff>
--- a/DATA/Pulsars_fluxes.xlsx
+++ b/DATA/Pulsars_fluxes.xlsx
@@ -47,18 +47,12 @@
     <t>DM B1133+16 GURT</t>
   </si>
   <si>
-    <t>SNR B0031-07 GURT</t>
-  </si>
-  <si>
     <t>SNR B0031-07 UTR2 full</t>
   </si>
   <si>
     <t>SNR B0031-07 UTR2 sect 01</t>
   </si>
   <si>
-    <t>SNR B0031-07 UTR2 sect 09</t>
-  </si>
-  <si>
     <t>DM B0031-07 UTR2 full</t>
   </si>
   <si>
@@ -183,6 +177,12 @@
   </si>
   <si>
     <t>temp resolution UTR2</t>
+  </si>
+  <si>
+    <t>SNR В0031-07 GURT</t>
+  </si>
+  <si>
+    <t>SNR В0031-07 UTR2 sect 09</t>
   </si>
 </sst>
 </file>
@@ -198,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +247,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -290,6 +296,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,8 +580,8 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E31" sqref="E31"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,28 +620,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>1</v>
@@ -655,45 +662,45 @@
         <v>6</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="12">
         <v>9.83</v>
@@ -707,7 +714,7 @@
       <c r="K2" s="7">
         <v>114.5</v>
       </c>
-      <c r="O2" s="7">
+      <c r="N2" s="9">
         <v>4.8491</v>
       </c>
       <c r="P2" s="5">
@@ -731,7 +738,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="12">
         <v>9.83</v>
@@ -745,7 +752,7 @@
       <c r="K3" s="7">
         <v>94.6</v>
       </c>
-      <c r="O3" s="7">
+      <c r="N3" s="9">
         <v>4.8491</v>
       </c>
       <c r="P3" s="5">
@@ -757,9 +764,6 @@
       <c r="U3" s="3">
         <v>19.625</v>
       </c>
-      <c r="V3" s="9">
-        <v>-1</v>
-      </c>
       <c r="W3" s="7">
         <v>202.4</v>
       </c>
@@ -769,7 +773,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="12">
         <v>9.83</v>
@@ -783,7 +787,7 @@
       <c r="K4" s="7">
         <v>178.1</v>
       </c>
-      <c r="O4" s="7">
+      <c r="N4" s="9">
         <v>4.8491</v>
       </c>
       <c r="P4" s="5">
@@ -807,7 +811,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="12">
         <v>9.83</v>
@@ -821,7 +825,7 @@
       <c r="K5" s="7">
         <v>217.6</v>
       </c>
-      <c r="O5" s="7">
+      <c r="N5" s="9">
         <v>4.8491</v>
       </c>
       <c r="P5" s="5">
@@ -845,7 +849,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="12">
         <v>9.83</v>
@@ -859,7 +863,7 @@
       <c r="K6" s="7">
         <v>62.8</v>
       </c>
-      <c r="O6" s="7">
+      <c r="N6" s="9">
         <v>4.8471000000000002</v>
       </c>
       <c r="P6" s="5">
@@ -883,7 +887,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="12">
         <v>9.83</v>
@@ -897,15 +901,9 @@
       <c r="K7" s="7">
         <v>188.5</v>
       </c>
-      <c r="O7" s="7">
-        <v>-1</v>
-      </c>
       <c r="Q7" s="3">
         <v>15.3</v>
       </c>
-      <c r="U7" s="3">
-        <v>-1</v>
-      </c>
       <c r="V7" s="9">
         <v>42</v>
       </c>
@@ -918,7 +916,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="12">
         <v>9.83</v>
@@ -932,7 +930,7 @@
       <c r="K8" s="7">
         <v>129.6</v>
       </c>
-      <c r="O8" s="7">
+      <c r="N8" s="9">
         <v>4.8471000000000002</v>
       </c>
       <c r="P8" s="5">
@@ -956,7 +954,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="12">
         <v>9.83</v>
@@ -970,7 +968,7 @@
       <c r="K9" s="7">
         <v>182.8</v>
       </c>
-      <c r="O9" s="7">
+      <c r="N9" s="9">
         <v>4.8471000000000002</v>
       </c>
       <c r="P9" s="5">
@@ -994,7 +992,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="12">
         <v>9.83</v>
@@ -1014,24 +1012,12 @@
       <c r="M10" s="7">
         <v>22.9</v>
       </c>
-      <c r="O10" s="7">
+      <c r="N10" s="9">
         <v>4.8471000000000002</v>
       </c>
       <c r="P10" s="5">
         <v>16.8</v>
       </c>
-      <c r="Q10" s="3">
-        <v>0</v>
-      </c>
-      <c r="R10" s="5">
-        <v>0</v>
-      </c>
-      <c r="S10" s="3">
-        <v>0</v>
-      </c>
-      <c r="U10" s="3">
-        <v>-1</v>
-      </c>
       <c r="V10" s="9">
         <v>46.9</v>
       </c>
@@ -1044,13 +1030,10 @@
       <c r="Y10" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AA10" s="7">
-        <v>-1</v>
-      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="12">
         <v>9.83</v>
@@ -1070,7 +1053,7 @@
       <c r="M11" s="7">
         <v>13.7</v>
       </c>
-      <c r="O11" s="7">
+      <c r="N11" s="9">
         <v>4.8491</v>
       </c>
       <c r="P11" s="5">
@@ -1100,13 +1083,10 @@
       <c r="Y11" s="7">
         <v>8.6</v>
       </c>
-      <c r="AA11" s="7">
-        <v>-1</v>
-      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="12">
         <v>9.83</v>
@@ -1126,7 +1106,7 @@
       <c r="M12" s="7">
         <v>17</v>
       </c>
-      <c r="O12" s="7">
+      <c r="N12" s="9">
         <v>4.8491</v>
       </c>
       <c r="P12" s="5">
@@ -1162,7 +1142,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="12">
         <v>9.83</v>
@@ -1182,7 +1162,7 @@
       <c r="M13" s="7">
         <v>15.8</v>
       </c>
-      <c r="O13" s="7">
+      <c r="N13" s="9">
         <v>4.8471000000000002</v>
       </c>
       <c r="Q13" s="3">
@@ -1191,15 +1171,6 @@
       <c r="R13" s="5">
         <v>5.2</v>
       </c>
-      <c r="S13" s="3">
-        <v>0</v>
-      </c>
-      <c r="U13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="V13" s="9">
-        <v>-1</v>
-      </c>
       <c r="W13" s="7">
         <v>236.9</v>
       </c>
@@ -1215,7 +1186,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="12">
         <v>9.83</v>
@@ -1235,24 +1206,12 @@
       <c r="M14" s="7">
         <v>16.8</v>
       </c>
-      <c r="O14" s="7">
-        <v>-1</v>
-      </c>
       <c r="Q14" s="3">
         <v>25.4</v>
       </c>
       <c r="R14" s="5">
         <v>5.2</v>
       </c>
-      <c r="S14" s="3">
-        <v>0</v>
-      </c>
-      <c r="U14" s="3">
-        <v>-1</v>
-      </c>
-      <c r="V14" s="9">
-        <v>-1</v>
-      </c>
       <c r="W14" s="7">
         <v>6.9</v>
       </c>
@@ -1262,13 +1221,10 @@
       <c r="Y14" s="7">
         <v>7.2</v>
       </c>
-      <c r="AA14" s="7">
-        <v>-1</v>
-      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="14">
         <v>7.94</v>
@@ -1276,7 +1232,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="14">
         <v>7.94</v>
@@ -1284,7 +1240,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="14">
         <v>7.94</v>
@@ -1292,7 +1248,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="14">
         <v>7.94</v>
@@ -1300,7 +1256,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="14">
         <v>7.94</v>
@@ -1308,7 +1264,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="14">
         <v>7.94</v>
@@ -1325,7 +1281,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21" s="14">
         <v>7.94</v>
@@ -1333,7 +1289,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="14">
         <v>7.94</v>
@@ -1341,7 +1297,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="14">
         <v>7.94</v>
@@ -1349,27 +1305,46 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="14">
         <v>7.94</v>
+      </c>
+      <c r="E24" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="F24" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="H24" s="5">
+        <v>10.896000000000001</v>
       </c>
       <c r="K24" s="7">
         <v>94.6</v>
       </c>
+      <c r="L24" s="9">
+        <v>16.100000000000001</v>
+      </c>
       <c r="N24" s="9">
         <v>4.8471000000000002</v>
       </c>
       <c r="Q24" s="3">
         <v>11.5</v>
       </c>
+      <c r="R24" s="5">
+        <v>17.8</v>
+      </c>
       <c r="T24" s="5">
         <v>19.623000000000001</v>
       </c>
+      <c r="W24" s="15"/>
+      <c r="X24" s="9">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="14">
         <v>7.94</v>
@@ -1413,7 +1388,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="14">
         <v>7.94</v>
@@ -1454,7 +1429,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" s="14">
         <v>7.94</v>

</xml_diff>

<commit_message>
added pulsars background plots
</commit_message>
<xml_diff>
--- a/DATA/Pulsars_fluxes.xlsx
+++ b/DATA/Pulsars_fluxes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PYTHON\jupyter-radio-astronomy\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\python\jupyter-radio-astronomy\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -89,9 +89,6 @@
     <t>SNR B1919+21 UTR2 sect 09</t>
   </si>
   <si>
-    <t>DM  B1919+21 UTR2 full</t>
-  </si>
-  <si>
     <t>DM B1919+21 GURT</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>SNR В0031-07 UTR2 sect 09</t>
+  </si>
+  <si>
+    <t>DM B1919+21 UTR2 full</t>
   </si>
 </sst>
 </file>
@@ -580,8 +580,8 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,13 +620,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
@@ -635,7 +635,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>9</v>
@@ -692,15 +692,15 @@
         <v>20</v>
       </c>
       <c r="Z1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="12">
         <v>9.83</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="12">
         <v>9.83</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="12">
         <v>9.83</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="12">
         <v>9.83</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="12">
         <v>9.83</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="12">
         <v>9.83</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="12">
         <v>9.83</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="12">
         <v>9.83</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="12">
         <v>9.83</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="12">
         <v>9.83</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="12">
         <v>9.83</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="12">
         <v>9.83</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="12">
         <v>9.83</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="14">
         <v>7.94</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="14">
         <v>7.94</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="14">
         <v>7.94</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="14">
         <v>7.94</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="14">
         <v>7.94</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="14">
         <v>7.94</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="14">
         <v>7.94</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="14">
         <v>7.94</v>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="14">
         <v>7.94</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="14">
         <v>7.94</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="14">
         <v>7.94</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="14">
         <v>7.94</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="14">
         <v>7.94</v>

</xml_diff>